<commit_message>
Updated progress on TAS verifications (spreadsheets)
Signed-off-by: bigbass1997 <bigbass1997.website@gmail.com>
</commit_message>
<xml_diff>
--- a/tas-verifications.xlsx
+++ b/tas-verifications.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="126">
   <si>
     <t xml:space="preserve">Publish ID</t>
   </si>
@@ -121,7 +121,7 @@
     <t xml:space="preserve">3179M</t>
   </si>
   <si>
-    <t xml:space="preserve">Focus</t>
+    <t xml:space="preserve">Planned</t>
   </si>
   <si>
     <t xml:space="preserve">Battletoads</t>
@@ -136,19 +136,16 @@
     <t xml:space="preserve">Gauntlet</t>
   </si>
   <si>
-    <t xml:space="preserve">It’s guantlet!</t>
+    <t xml:space="preserve">It’s guantlet! Desyncs inconsistently</t>
   </si>
   <si>
     <t xml:space="preserve">4349M</t>
   </si>
   <si>
-    <t xml:space="preserve">Planned</t>
-  </si>
-  <si>
     <t xml:space="preserve">Marble Madness</t>
   </si>
   <si>
-    <t xml:space="preserve">Madness indeed…</t>
+    <t xml:space="preserve">Desyncs consistently, ball moves too far to the left and falls off the platform on first level.</t>
   </si>
   <si>
     <t xml:space="preserve">4386M</t>
@@ -157,7 +154,7 @@
     <t xml:space="preserve">Batman</t>
   </si>
   <si>
-    <t xml:space="preserve">Last verified in 2008!</t>
+    <t xml:space="preserve">TheDot said this verifies, but I experience consistent desyncs.</t>
   </si>
   <si>
     <t xml:space="preserve">4104M</t>
@@ -187,12 +184,12 @@
     <t xml:space="preserve">Zelda II: The Adventure of Link</t>
   </si>
   <si>
-    <t xml:space="preserve">Previous verifications may be false!</t>
-  </si>
-  <si>
     <t xml:space="preserve">4234M</t>
   </si>
   <si>
+    <t xml:space="preserve">warp glitch</t>
+  </si>
+  <si>
     <t xml:space="preserve">4226M</t>
   </si>
   <si>
@@ -235,10 +232,172 @@
     <t xml:space="preserve">Another playaround category; plus it’s football!</t>
   </si>
   <si>
-    <t xml:space="preserve">1649M</t>
+    <t xml:space="preserve">4410M</t>
   </si>
   <si>
     <t xml:space="preserve">Mega Man 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desyncs on Woodman stage, first screen transition glitch. Glitch is performed slightly differently on this compared to older verification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2652M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Previously verified but lacked video evidence until now</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3254M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">warpless</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1956M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ghostbusters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desyncs, inconsistent enemies (possibly needs initial RAM set)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1421M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wizardry II</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Requires cartridge in order to start playback without resetting (might be able to start from everdrive menu if proper inputs prepended)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1352M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Donkey Kong</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desyncs, unknown cause</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2792M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Great Waldo Search</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3591M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">North and South</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2211M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Archon: The Light and the Dark</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Different RNG, but consistent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2699M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Priority</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hydlide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Must start from power-on/everdrive-menu. Reset vector is after the splash screen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">744M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jaws</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desyncs consistently, after player goes diving the enemies are consisten, but not in the same positions as the encoded video. (+1/+2 frame doesn’t change anything)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1825M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pinball Quest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desyncs consistently, after talking with the ghost. Ball is hit into the left tree and then drains.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3194M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mini Putt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desyncs, inconsistently</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1228M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">High Speed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desyncs, immediately. Might be wrong ROM or needs blank frames.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1915M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indiana Jones and the Last Crusade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desyncs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3135M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cosmo Police: Galivan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3995M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strider</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desyncs, at first significant screen glitch.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3943M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arkanoid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Required ViGreyTech’s fixed dump script</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3613M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bionic Commando</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desyncs consistently, at 8:52 in encoded video. Menu option should be right to “Transfer” but doesn’t.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3028M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Super Mario Bros. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desyncs. And a different verified run also desyncs. Possible problem with replay device.</t>
   </si>
 </sst>
 </file>
@@ -563,10 +722,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ24"/>
+  <dimension ref="A1:AMJ43"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
+      <selection pane="topLeft" activeCell="A45" activeCellId="0" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -575,7 +734,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="53.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="17.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="99.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="142.28"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="6" style="4" width="11.52"/>
   </cols>
   <sheetData>
@@ -734,7 +893,7 @@
         <v>36</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>37</v>
@@ -751,178 +910,501 @@
         <v>39</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>49</v>
+      <c r="E15" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>55</v>
+      <c r="D17" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>40</v>
+        <v>6</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E18" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>58</v>
+      <c r="D19" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C21" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" s="2" t="s">
+      <c r="D22" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="E22" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C23" s="2" t="s">
+      <c r="D23" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C24" s="2" t="s">
+      <c r="D24" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>24</v>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update progress on TAS verifications, again...
Signed-off-by: bigbass1997 <bigbass1997.website@gmail.com>
</commit_message>
<xml_diff>
--- a/tas-verifications.xlsx
+++ b/tas-verifications.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="143">
   <si>
     <t xml:space="preserve">Publish ID</t>
   </si>
@@ -244,7 +244,7 @@
     <t xml:space="preserve">2652M</t>
   </si>
   <si>
-    <t xml:space="preserve">Previously verified but lacked video evidence until now</t>
+    <t xml:space="preserve">2021-03-25 Previously verified but lacked video evidence until now</t>
   </si>
   <si>
     <t xml:space="preserve">3254M</t>
@@ -379,7 +379,7 @@
     <t xml:space="preserve">Arkanoid</t>
   </si>
   <si>
-    <t xml:space="preserve">Required ViGreyTech’s fixed dump script</t>
+    <t xml:space="preserve">2021-03-29 Required ViGreyTech’s fixed dump script</t>
   </si>
   <si>
     <t xml:space="preserve">3613M</t>
@@ -398,14 +398,67 @@
   </si>
   <si>
     <t xml:space="preserve">Desyncs. And a different verified run also desyncs. Possible problem with replay device.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2422M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Streemerz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Superb Joe mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desyncs semi-consistent. If it reaches first level, it desyncs exactly like “New PPU” mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2923M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Streeeeemerz mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desyncs consistently. Either selects wrong options if SRAM isn’t clear. Or desyncs at 2:35 (encode time).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3726M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Super C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 players</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4353M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ninja Gaiden II: The Dark Sword of Chaos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2421M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Battle City</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1546M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gimmick!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -552,7 +605,7 @@
     <xf numFmtId="164" fontId="0" fillId="6" borderId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -581,8 +634,16 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -722,10 +783,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ43"/>
+  <dimension ref="A1:AMJ49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A45" activeCellId="0" sqref="A45"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E55" activeCellId="0" sqref="E55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -769,6 +830,9 @@
       <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="E2" s="7" t="n">
+        <v>44245</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
@@ -783,6 +847,9 @@
       <c r="D3" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="E3" s="7" t="n">
+        <v>44246</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
@@ -811,6 +878,9 @@
       <c r="D5" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="E5" s="7" t="n">
+        <v>44251</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
@@ -873,6 +943,9 @@
       <c r="D9" s="3" t="s">
         <v>31</v>
       </c>
+      <c r="E9" s="7" t="n">
+        <v>44251</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
@@ -889,7 +962,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="8" t="s">
         <v>36</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -988,6 +1061,9 @@
       <c r="D17" s="3" t="s">
         <v>24</v>
       </c>
+      <c r="E17" s="7" t="n">
+        <v>44282</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
@@ -1002,6 +1078,9 @@
       <c r="D18" s="3" t="s">
         <v>55</v>
       </c>
+      <c r="E18" s="7" t="n">
+        <v>44281</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
@@ -1016,6 +1095,9 @@
       <c r="D19" s="3" t="s">
         <v>24</v>
       </c>
+      <c r="E19" s="7" t="n">
+        <v>44284</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
@@ -1123,6 +1205,9 @@
       <c r="D26" s="3" t="s">
         <v>76</v>
       </c>
+      <c r="E26" s="7" t="n">
+        <v>44280</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
@@ -1188,6 +1273,9 @@
       <c r="D30" s="3" t="s">
         <v>24</v>
       </c>
+      <c r="E30" s="7" t="n">
+        <v>44282</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
@@ -1202,6 +1290,9 @@
       <c r="D31" s="3" t="s">
         <v>24</v>
       </c>
+      <c r="E31" s="7" t="n">
+        <v>44282</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
@@ -1405,6 +1496,108 @@
       </c>
       <c r="E43" s="2" t="s">
         <v>125</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E47" s="7" t="n">
+        <v>44285</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>